<commit_message>
Github actions workflow update for Egrants
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/RASScenario1.xlsx
+++ b/src/test/java/CHARMS/resources/RASScenario1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E3E624-CFC9-724D-92E7-9551D40421D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12825D8-A455-584F-948D-EB9CC4C8D1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="1000" windowWidth="22940" windowHeight="14300" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
+    <workbookView xWindow="5040" yWindow="1000" windowWidth="22940" windowHeight="14300" activeTab="1" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="337">
   <si>
     <t>Question</t>
   </si>
@@ -1120,6 +1120,14 @@
   </si>
   <si>
     <t>October</t>
+  </si>
+  <si>
+    <t>This questionnaire should take you approximately 30 minutes to complete. It does not need to be completed all at once.
+We encourage you to take a break and return to complete the survey later, if needed.
+You can save your answers by clicking the "Save and Next" button in the survey and closing your browser window.
+When you return to the survey, you will be asked for a PIN code, provided during the log in process.
+This unique PIN code returns you to your previous spot in the questionnaire.
+The study team requests that you complete the questionnaire within two months from the date you start the questionnaire.</t>
   </si>
 </sst>
 </file>
@@ -1549,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA49E6-03DB-BC47-B34D-065780B05137}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1855,10 +1863,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA38AB1-F752-BB4E-9CFB-C6D8167B319F}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1892,33 +1900,33 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="187" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B5" s="9" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
@@ -1926,39 +1934,39 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>14</v>
@@ -1966,151 +1974,151 @@
     </row>
     <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="4">
-        <v>10</v>
+        <v>116</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B16" s="4">
         <v>2004</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B17" s="6">
         <v>38301</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>66</v>
+        <v>97</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>14</v>
@@ -2118,7 +2126,7 @@
     </row>
     <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>14</v>
@@ -2126,79 +2134,79 @@
     </row>
     <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34" s="4">
-        <v>4.5</v>
+        <v>84</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="4">
-        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B37" s="4">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>87</v>
+        <v>108</v>
+      </c>
+      <c r="B38" s="4">
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
+    <row r="41" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>14</v>
@@ -2206,71 +2214,71 @@
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="4">
-        <v>70</v>
+        <v>111</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="B45" s="4">
-        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B46" s="4">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B47" s="4">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B48" s="4">
-        <v>100</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B49" s="4">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>86</v>
+        <v>270</v>
+      </c>
+      <c r="B50" s="4">
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>86</v>
@@ -2278,7 +2286,7 @@
     </row>
     <row r="52" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>86</v>
@@ -2286,57 +2294,65 @@
     </row>
     <row r="53" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>276</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>89</v>
+        <v>275</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>63</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="136" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+      <c r="B59" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B60" s="8" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2349,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89138E5-4B7A-8A4C-A60B-54B878E1BA10}">
   <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>